<commit_message>
[Subject] 1.0612 [Bug Number/CSP Number/Enhancement/New Feature] N/A [Ripple Effect] N/A [Solution] N/A [Project]
</commit_message>
<xml_diff>
--- a/APP/Codes/Driver/GPIO.xlsx
+++ b/APP/Codes/Driver/GPIO.xlsx
@@ -10,14 +10,14 @@
     <sheet name="IO" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$2:$F$91</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">IO!$A$2:$F$142</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1007" uniqueCount="185">
   <si>
     <t>Wakeup</t>
   </si>
@@ -385,13 +385,28 @@
     <t>PF6</t>
   </si>
   <si>
+    <t>IO_F_CS</t>
+  </si>
+  <si>
     <t>PF7</t>
   </si>
   <si>
+    <t>IO_SPI5_SCK</t>
+  </si>
+  <si>
+    <t>GPIO_AF5</t>
+  </si>
+  <si>
     <t>PF8</t>
   </si>
   <si>
+    <t>IO_SPI5_MISO</t>
+  </si>
+  <si>
     <t>PF9</t>
+  </si>
+  <si>
+    <t>IO_SPI5_MOSI</t>
   </si>
   <si>
     <t>PF10</t>
@@ -565,11 +580,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -594,7 +609,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -602,6 +624,35 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -616,24 +667,17 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -646,13 +690,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="等线"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="等线"/>
@@ -675,6 +720,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="等线"/>
@@ -690,17 +743,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="等线"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -713,31 +757,8 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="36">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -753,12 +774,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -812,7 +827,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -824,7 +851,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -836,13 +887,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -854,13 +929,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -872,79 +959,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1113,6 +1128,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1143,6 +1182,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1154,39 +1202,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1218,10 +1233,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1230,133 +1245,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1400,64 +1415,64 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1784,7 +1799,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E101" sqref="E101"/>
+      <selection pane="bottomLeft" activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1806,7 +1821,7 @@
     <col min="16" max="16" width="12.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" ht="15" spans="1:18">
       <c r="A1" s="3"/>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -1818,8 +1833,8 @@
       <c r="G1" s="7"/>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="21"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
       <c r="N1" s="12"/>
@@ -1856,10 +1871,10 @@
       <c r="I2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="23"/>
+      <c r="K2" s="22"/>
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
       <c r="N2" s="12"/>
@@ -1896,8 +1911,8 @@
       <c r="I3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="24"/>
-      <c r="K3" s="25"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="24"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
       <c r="N3" s="12"/>
@@ -1913,7 +1928,7 @@
       <c r="B4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="13"/>
+      <c r="C4" s="10"/>
       <c r="D4" s="11" t="s">
         <v>20</v>
       </c>
@@ -1932,8 +1947,8 @@
       <c r="I4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
+      <c r="J4" s="23"/>
+      <c r="K4" s="24"/>
       <c r="L4" s="12"/>
       <c r="M4" s="12"/>
       <c r="N4" s="12"/>
@@ -1949,7 +1964,7 @@
       <c r="B5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="13"/>
+      <c r="C5" s="10"/>
       <c r="D5" s="11" t="s">
         <v>20</v>
       </c>
@@ -1968,8 +1983,8 @@
       <c r="I5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="24"/>
-      <c r="K5" s="25"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="24"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
@@ -1985,7 +2000,7 @@
       <c r="B6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="13"/>
+      <c r="C6" s="10"/>
       <c r="D6" s="11" t="s">
         <v>20</v>
       </c>
@@ -2004,8 +2019,8 @@
       <c r="I6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="25"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="24"/>
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="12"/>
@@ -2040,8 +2055,8 @@
       <c r="I7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="25"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
@@ -2076,8 +2091,8 @@
       <c r="I8" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="25"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="24"/>
       <c r="L8" s="12"/>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
@@ -2112,8 +2127,8 @@
       <c r="I9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="25"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="24"/>
       <c r="L9" s="12"/>
       <c r="M9" s="12"/>
       <c r="N9" s="12"/>
@@ -2129,7 +2144,7 @@
       <c r="B10" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="10"/>
       <c r="D10" s="11" t="s">
         <v>20</v>
       </c>
@@ -2148,8 +2163,8 @@
       <c r="I10" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="24"/>
-      <c r="K10" s="25"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="24"/>
       <c r="L10" s="12"/>
       <c r="M10" s="12"/>
       <c r="N10" s="12"/>
@@ -2184,8 +2199,8 @@
       <c r="I11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="24"/>
       <c r="L11" s="12"/>
       <c r="M11" s="12"/>
       <c r="N11" s="12"/>
@@ -2222,8 +2237,8 @@
       <c r="I12" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="24"/>
       <c r="L12" s="12"/>
       <c r="M12" s="12"/>
       <c r="N12" s="12"/>
@@ -2260,8 +2275,8 @@
       <c r="I13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="24"/>
       <c r="L13" s="12"/>
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
@@ -2298,8 +2313,8 @@
       <c r="I14" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="25"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="24"/>
       <c r="L14" s="12"/>
       <c r="M14" s="12"/>
       <c r="N14" s="12"/>
@@ -2336,8 +2351,8 @@
       <c r="I15" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="24"/>
       <c r="L15" s="12"/>
       <c r="M15" s="12"/>
       <c r="N15" s="12"/>
@@ -2372,8 +2387,8 @@
       <c r="I16" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="25"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="24"/>
       <c r="L16" s="12"/>
       <c r="M16" s="12"/>
       <c r="N16" s="12"/>
@@ -2408,8 +2423,8 @@
       <c r="I17" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J17" s="24"/>
-      <c r="K17" s="25"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="24"/>
       <c r="L17" s="12"/>
       <c r="M17" s="12"/>
       <c r="N17" s="12"/>
@@ -2444,8 +2459,8 @@
       <c r="I18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="24"/>
-      <c r="K18" s="25"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="24"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
       <c r="N18" s="12"/>
@@ -2455,10 +2470,10 @@
       <c r="R18" s="11"/>
     </row>
     <row r="19" s="1" customFormat="1" spans="1:18">
-      <c r="A19" s="14">
-        <v>22</v>
-      </c>
-      <c r="B19" s="15" t="s">
+      <c r="A19" s="13">
+        <v>22</v>
+      </c>
+      <c r="B19" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="10" t="s">
@@ -2467,7 +2482,7 @@
       <c r="D19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E19" s="16" t="s">
+      <c r="E19" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F19" s="12" t="s">
@@ -2479,24 +2494,24 @@
       <c r="H19" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" s="26"/>
-      <c r="K19" s="27"/>
+      <c r="I19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="25"/>
+      <c r="K19" s="26"/>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10"/>
       <c r="O19" s="10"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="16"/>
-      <c r="R19" s="16"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
     </row>
     <row r="20" ht="12" customHeight="1" spans="1:18">
       <c r="A20" s="3">
         <v>23</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="14" t="s">
         <v>49</v>
       </c>
       <c r="C20" s="10" t="s">
@@ -2520,8 +2535,8 @@
       <c r="I20" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J20" s="24"/>
-      <c r="K20" s="25"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="24"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
@@ -2531,17 +2546,17 @@
       <c r="R20" s="11"/>
     </row>
     <row r="21" s="1" customFormat="1" spans="1:18">
-      <c r="A21" s="14">
+      <c r="A21" s="13">
         <v>24</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="14" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F21" s="12" t="s">
@@ -2553,31 +2568,31 @@
       <c r="H21" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I21" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="26"/>
-      <c r="K21" s="27"/>
+      <c r="I21" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="25"/>
+      <c r="K21" s="26"/>
       <c r="L21" s="10"/>
       <c r="M21" s="10"/>
       <c r="N21" s="10"/>
       <c r="O21" s="10"/>
-      <c r="P21" s="16"/>
-      <c r="Q21" s="16"/>
-      <c r="R21" s="16"/>
+      <c r="P21" s="15"/>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15"/>
     </row>
     <row r="22" s="1" customFormat="1" spans="1:18">
-      <c r="A22" s="14">
+      <c r="A22" s="13">
         <v>25</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="14" t="s">
         <v>52</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="16" t="s">
+      <c r="E22" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F22" s="12" t="s">
@@ -2589,31 +2604,31 @@
       <c r="H22" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I22" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
+      <c r="I22" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="25"/>
+      <c r="K22" s="26"/>
       <c r="L22" s="10"/>
       <c r="M22" s="10"/>
       <c r="N22" s="10"/>
       <c r="O22" s="10"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="16"/>
-      <c r="R22" s="16"/>
+      <c r="P22" s="15"/>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15"/>
     </row>
     <row r="23" s="1" customFormat="1" ht="12.75" customHeight="1" spans="1:18">
-      <c r="A23" s="14">
+      <c r="A23" s="13">
         <v>26</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="14" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E23" s="16" t="s">
+      <c r="E23" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F23" s="12" t="s">
@@ -2625,31 +2640,31 @@
       <c r="H23" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="16" t="s">
+      <c r="I23" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
+      <c r="J23" s="25"/>
+      <c r="K23" s="26"/>
       <c r="L23" s="10"/>
       <c r="M23" s="10"/>
       <c r="N23" s="10"/>
       <c r="O23" s="10"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="16"/>
-      <c r="R23" s="16"/>
+      <c r="P23" s="15"/>
+      <c r="Q23" s="15"/>
+      <c r="R23" s="15"/>
     </row>
     <row r="24" s="1" customFormat="1" spans="1:18">
-      <c r="A24" s="14">
+      <c r="A24" s="13">
         <v>27</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F24" s="12" t="s">
@@ -2661,31 +2676,31 @@
       <c r="H24" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I24" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="26"/>
-      <c r="K24" s="27"/>
+      <c r="I24" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="26"/>
       <c r="L24" s="10"/>
       <c r="M24" s="10"/>
       <c r="N24" s="10"/>
       <c r="O24" s="10"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
+      <c r="P24" s="15"/>
+      <c r="Q24" s="15"/>
+      <c r="R24" s="15"/>
     </row>
     <row r="25" s="1" customFormat="1" spans="1:18">
-      <c r="A25" s="14">
+      <c r="A25" s="13">
         <v>28</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="14" t="s">
         <v>55</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F25" s="12" t="s">
@@ -2697,31 +2712,31 @@
       <c r="H25" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I25" s="16" t="s">
+      <c r="I25" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="J25" s="26"/>
-      <c r="K25" s="27"/>
+      <c r="J25" s="25"/>
+      <c r="K25" s="26"/>
       <c r="L25" s="10"/>
       <c r="M25" s="10"/>
       <c r="N25" s="10"/>
       <c r="O25" s="10"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="16"/>
+      <c r="P25" s="15"/>
+      <c r="Q25" s="15"/>
+      <c r="R25" s="15"/>
     </row>
     <row r="26" s="1" customFormat="1" spans="1:18">
-      <c r="A26" s="14">
+      <c r="A26" s="13">
         <v>29</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="16" t="s">
+      <c r="E26" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F26" s="12" t="s">
@@ -2733,24 +2748,24 @@
       <c r="H26" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="26"/>
-      <c r="K26" s="27"/>
+      <c r="I26" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="25"/>
+      <c r="K26" s="26"/>
       <c r="L26" s="10"/>
       <c r="M26" s="10"/>
       <c r="N26" s="10"/>
       <c r="O26" s="10"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
+      <c r="P26" s="15"/>
+      <c r="Q26" s="15"/>
+      <c r="R26" s="15"/>
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="3">
         <v>30</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="14" t="s">
         <v>58</v>
       </c>
       <c r="C27" s="12"/>
@@ -2772,8 +2787,8 @@
       <c r="I27" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J27" s="24"/>
-      <c r="K27" s="25"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="24"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
@@ -2783,17 +2798,17 @@
       <c r="R27" s="11"/>
     </row>
     <row r="28" s="1" customFormat="1" spans="1:18">
-      <c r="A28" s="14">
+      <c r="A28" s="13">
         <v>31</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="14" t="s">
         <v>59</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F28" s="12" t="s">
@@ -2805,24 +2820,24 @@
       <c r="H28" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="26"/>
-      <c r="K28" s="27"/>
+      <c r="I28" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="25"/>
+      <c r="K28" s="26"/>
       <c r="L28" s="10"/>
       <c r="M28" s="10"/>
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="16"/>
-      <c r="R28" s="16"/>
+      <c r="P28" s="15"/>
+      <c r="Q28" s="15"/>
+      <c r="R28" s="15"/>
     </row>
     <row r="29" spans="1:18">
       <c r="A29" s="3">
         <v>32</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="14" t="s">
         <v>60</v>
       </c>
       <c r="C29" s="12"/>
@@ -2844,8 +2859,8 @@
       <c r="I29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J29" s="24"/>
-      <c r="K29" s="25"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="24"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12"/>
       <c r="N29" s="12"/>
@@ -2855,17 +2870,17 @@
       <c r="R29" s="11"/>
     </row>
     <row r="30" s="1" customFormat="1" spans="1:18">
-      <c r="A30" s="14">
+      <c r="A30" s="13">
         <v>33</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="10"/>
-      <c r="D30" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E30" s="16" t="s">
+      <c r="D30" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E30" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F30" s="12" t="s">
@@ -2877,31 +2892,31 @@
       <c r="H30" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I30" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="26"/>
-      <c r="K30" s="27"/>
+      <c r="I30" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="25"/>
+      <c r="K30" s="26"/>
       <c r="L30" s="10"/>
       <c r="M30" s="10"/>
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="16"/>
-      <c r="R30" s="16"/>
+      <c r="P30" s="15"/>
+      <c r="Q30" s="15"/>
+      <c r="R30" s="15"/>
     </row>
     <row r="31" s="1" customFormat="1" spans="1:18">
-      <c r="A31" s="14">
+      <c r="A31" s="13">
         <v>34</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="14" t="s">
         <v>62</v>
       </c>
       <c r="C31" s="10"/>
-      <c r="D31" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E31" s="16" t="s">
+      <c r="D31" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E31" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F31" s="12" t="s">
@@ -2913,31 +2928,31 @@
       <c r="H31" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="26"/>
-      <c r="K31" s="27"/>
+      <c r="I31" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="25"/>
+      <c r="K31" s="26"/>
       <c r="L31" s="10"/>
       <c r="M31" s="10"/>
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="16"/>
-      <c r="R31" s="16"/>
+      <c r="P31" s="15"/>
+      <c r="Q31" s="15"/>
+      <c r="R31" s="15"/>
     </row>
     <row r="32" s="1" customFormat="1" spans="1:18">
-      <c r="A32" s="14">
+      <c r="A32" s="13">
         <v>35</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C32" s="10"/>
-      <c r="D32" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="16" t="s">
+      <c r="D32" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E32" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="12" t="s">
@@ -2949,24 +2964,24 @@
       <c r="H32" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="26"/>
-      <c r="K32" s="27"/>
+      <c r="I32" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="25"/>
+      <c r="K32" s="26"/>
       <c r="L32" s="10"/>
       <c r="M32" s="10"/>
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="16"/>
-      <c r="R32" s="16"/>
+      <c r="P32" s="15"/>
+      <c r="Q32" s="15"/>
+      <c r="R32" s="15"/>
     </row>
     <row r="33" spans="1:18">
       <c r="A33" s="3">
         <v>36</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="14" t="s">
         <v>64</v>
       </c>
       <c r="C33" s="12"/>
@@ -2988,8 +3003,8 @@
       <c r="I33" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J33" s="24"/>
-      <c r="K33" s="25"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="24"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
       <c r="N33" s="12"/>
@@ -2999,17 +3014,17 @@
       <c r="R33" s="11"/>
     </row>
     <row r="34" s="1" customFormat="1" spans="1:18">
-      <c r="A34" s="14">
+      <c r="A34" s="13">
         <v>39</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="14" t="s">
         <v>65</v>
       </c>
       <c r="C34" s="10"/>
-      <c r="D34" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="16" t="s">
+      <c r="D34" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F34" s="12" t="s">
@@ -3021,24 +3036,24 @@
       <c r="H34" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" s="26"/>
-      <c r="K34" s="27"/>
+      <c r="I34" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" s="25"/>
+      <c r="K34" s="26"/>
       <c r="L34" s="10"/>
       <c r="M34" s="10"/>
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="16"/>
-      <c r="R34" s="16"/>
+      <c r="P34" s="15"/>
+      <c r="Q34" s="15"/>
+      <c r="R34" s="15"/>
     </row>
     <row r="35" spans="1:18">
       <c r="A35" s="3">
         <v>40</v>
       </c>
-      <c r="B35" s="17" t="s">
+      <c r="B35" s="16" t="s">
         <v>66</v>
       </c>
       <c r="C35" s="12"/>
@@ -3060,8 +3075,8 @@
       <c r="I35" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J35" s="24"/>
-      <c r="K35" s="25"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="24"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
       <c r="N35" s="12"/>
@@ -3071,17 +3086,17 @@
       <c r="R35" s="11"/>
     </row>
     <row r="36" s="1" customFormat="1" spans="1:18">
-      <c r="A36" s="14">
+      <c r="A36" s="13">
         <v>41</v>
       </c>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="16" t="s">
         <v>67</v>
       </c>
       <c r="C36" s="10"/>
-      <c r="D36" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" s="16" t="s">
+      <c r="D36" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E36" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F36" s="12" t="s">
@@ -3093,31 +3108,31 @@
       <c r="H36" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I36" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J36" s="26"/>
-      <c r="K36" s="27"/>
+      <c r="I36" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="25"/>
+      <c r="K36" s="26"/>
       <c r="L36" s="10"/>
       <c r="M36" s="10"/>
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
-      <c r="P36" s="16"/>
-      <c r="Q36" s="16"/>
-      <c r="R36" s="16"/>
+      <c r="P36" s="15"/>
+      <c r="Q36" s="15"/>
+      <c r="R36" s="15"/>
     </row>
     <row r="37" s="1" customFormat="1" spans="1:18">
-      <c r="A37" s="14">
+      <c r="A37" s="13">
         <v>42</v>
       </c>
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="16" t="s">
         <v>68</v>
       </c>
       <c r="C37" s="10"/>
-      <c r="D37" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E37" s="16" t="s">
+      <c r="D37" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E37" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F37" s="12" t="s">
@@ -3129,31 +3144,31 @@
       <c r="H37" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I37" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J37" s="26"/>
-      <c r="K37" s="27"/>
+      <c r="I37" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="25"/>
+      <c r="K37" s="26"/>
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
-      <c r="P37" s="16"/>
-      <c r="Q37" s="16"/>
-      <c r="R37" s="16"/>
+      <c r="P37" s="15"/>
+      <c r="Q37" s="15"/>
+      <c r="R37" s="15"/>
     </row>
     <row r="38" s="1" customFormat="1" spans="1:18">
-      <c r="A38" s="14">
+      <c r="A38" s="13">
         <v>43</v>
       </c>
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="16" t="s">
         <v>69</v>
       </c>
       <c r="C38" s="10"/>
-      <c r="D38" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E38" s="16" t="s">
+      <c r="D38" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F38" s="12" t="s">
@@ -3165,24 +3180,24 @@
       <c r="H38" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I38" s="16" t="s">
+      <c r="I38" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J38" s="26"/>
-      <c r="K38" s="27"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="26"/>
       <c r="L38" s="10"/>
       <c r="M38" s="10"/>
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
-      <c r="P38" s="16"/>
-      <c r="Q38" s="16"/>
-      <c r="R38" s="16"/>
+      <c r="P38" s="15"/>
+      <c r="Q38" s="15"/>
+      <c r="R38" s="15"/>
     </row>
     <row r="39" spans="1:18">
       <c r="A39" s="3">
         <v>44</v>
       </c>
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="16" t="s">
         <v>70</v>
       </c>
       <c r="C39" s="12"/>
@@ -3204,8 +3219,8 @@
       <c r="I39" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J39" s="24"/>
-      <c r="K39" s="25"/>
+      <c r="J39" s="23"/>
+      <c r="K39" s="24"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
       <c r="N39" s="12"/>
@@ -3218,7 +3233,7 @@
       <c r="A40" s="3">
         <v>45</v>
       </c>
-      <c r="B40" s="17" t="s">
+      <c r="B40" s="16" t="s">
         <v>71</v>
       </c>
       <c r="C40" s="12"/>
@@ -3240,8 +3255,8 @@
       <c r="I40" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J40" s="24"/>
-      <c r="K40" s="25"/>
+      <c r="J40" s="23"/>
+      <c r="K40" s="24"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
       <c r="N40" s="12"/>
@@ -3251,17 +3266,17 @@
       <c r="R40" s="11"/>
     </row>
     <row r="41" s="1" customFormat="1" spans="1:18">
-      <c r="A41" s="14">
+      <c r="A41" s="13">
         <v>46</v>
       </c>
-      <c r="B41" s="17" t="s">
+      <c r="B41" s="16" t="s">
         <v>72</v>
       </c>
       <c r="C41" s="10"/>
-      <c r="D41" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E41" s="16" t="s">
+      <c r="D41" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E41" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F41" s="12" t="s">
@@ -3273,24 +3288,24 @@
       <c r="H41" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I41" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J41" s="26"/>
-      <c r="K41" s="27"/>
+      <c r="I41" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J41" s="25"/>
+      <c r="K41" s="26"/>
       <c r="L41" s="10"/>
       <c r="M41" s="10"/>
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
-      <c r="P41" s="16"/>
-      <c r="Q41" s="16"/>
-      <c r="R41" s="16"/>
+      <c r="P41" s="15"/>
+      <c r="Q41" s="15"/>
+      <c r="R41" s="15"/>
     </row>
     <row r="42" spans="1:18">
       <c r="A42" s="3">
         <v>47</v>
       </c>
-      <c r="B42" s="17" t="s">
+      <c r="B42" s="16" t="s">
         <v>73</v>
       </c>
       <c r="C42" s="12"/>
@@ -3312,8 +3327,8 @@
       <c r="I42" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J42" s="24"/>
-      <c r="K42" s="25"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="24"/>
       <c r="L42" s="12"/>
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
@@ -3323,17 +3338,17 @@
       <c r="R42" s="11"/>
     </row>
     <row r="43" s="1" customFormat="1" spans="1:18">
-      <c r="A43" s="14">
+      <c r="A43" s="13">
         <v>48</v>
       </c>
-      <c r="B43" s="17" t="s">
+      <c r="B43" s="16" t="s">
         <v>74</v>
       </c>
       <c r="C43" s="10"/>
-      <c r="D43" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E43" s="16" t="s">
+      <c r="D43" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F43" s="12" t="s">
@@ -3345,24 +3360,24 @@
       <c r="H43" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I43" s="16" t="s">
+      <c r="I43" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J43" s="26"/>
-      <c r="K43" s="27"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="26"/>
       <c r="L43" s="10"/>
       <c r="M43" s="10"/>
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
-      <c r="P43" s="16"/>
-      <c r="Q43" s="16"/>
-      <c r="R43" s="16"/>
+      <c r="P43" s="15"/>
+      <c r="Q43" s="15"/>
+      <c r="R43" s="15"/>
     </row>
     <row r="44" spans="1:18">
       <c r="A44" s="3">
         <v>49</v>
       </c>
-      <c r="B44" s="17" t="s">
+      <c r="B44" s="16" t="s">
         <v>75</v>
       </c>
       <c r="C44" s="12"/>
@@ -3384,8 +3399,8 @@
       <c r="I44" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J44" s="24"/>
-      <c r="K44" s="25"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="24"/>
       <c r="L44" s="12"/>
       <c r="M44" s="12"/>
       <c r="N44" s="12"/>
@@ -3398,7 +3413,7 @@
       <c r="A45" s="3">
         <v>50</v>
       </c>
-      <c r="B45" s="17" t="s">
+      <c r="B45" s="16" t="s">
         <v>76</v>
       </c>
       <c r="C45" s="12"/>
@@ -3420,8 +3435,8 @@
       <c r="I45" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J45" s="24"/>
-      <c r="K45" s="25"/>
+      <c r="J45" s="23"/>
+      <c r="K45" s="24"/>
       <c r="L45" s="12"/>
       <c r="M45" s="12"/>
       <c r="N45" s="12"/>
@@ -3434,7 +3449,7 @@
       <c r="A46" s="3">
         <v>51</v>
       </c>
-      <c r="B46" s="17" t="s">
+      <c r="B46" s="16" t="s">
         <v>77</v>
       </c>
       <c r="C46" s="12"/>
@@ -3456,8 +3471,8 @@
       <c r="I46" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J46" s="24"/>
-      <c r="K46" s="25"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="24"/>
       <c r="L46" s="12"/>
       <c r="M46" s="12"/>
       <c r="N46" s="12"/>
@@ -3467,17 +3482,17 @@
       <c r="R46" s="11"/>
     </row>
     <row r="47" s="1" customFormat="1" spans="1:18">
-      <c r="A47" s="14">
+      <c r="A47" s="13">
         <v>52</v>
       </c>
-      <c r="B47" s="17" t="s">
+      <c r="B47" s="16" t="s">
         <v>78</v>
       </c>
       <c r="C47" s="10"/>
-      <c r="D47" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E47" s="16" t="s">
+      <c r="D47" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E47" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F47" s="12" t="s">
@@ -3489,33 +3504,33 @@
       <c r="H47" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I47" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J47" s="26"/>
-      <c r="K47" s="27"/>
+      <c r="I47" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J47" s="25"/>
+      <c r="K47" s="26"/>
       <c r="L47" s="10"/>
       <c r="M47" s="10"/>
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="16"/>
-      <c r="R47" s="16"/>
+      <c r="P47" s="15"/>
+      <c r="Q47" s="15"/>
+      <c r="R47" s="15"/>
     </row>
     <row r="48" s="1" customFormat="1" spans="1:18">
-      <c r="A48" s="14">
+      <c r="A48" s="13">
         <v>53</v>
       </c>
-      <c r="B48" s="17" t="s">
+      <c r="B48" s="16" t="s">
         <v>79</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E48" s="16" t="s">
+      <c r="E48" s="15" t="s">
         <v>33</v>
       </c>
       <c r="F48" s="12" t="s">
@@ -3527,31 +3542,31 @@
       <c r="H48" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I48" s="16" t="s">
+      <c r="I48" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J48" s="26"/>
-      <c r="K48" s="27"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="26"/>
       <c r="L48" s="10"/>
       <c r="M48" s="10"/>
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
-      <c r="P48" s="16"/>
-      <c r="Q48" s="16"/>
-      <c r="R48" s="16"/>
+      <c r="P48" s="15"/>
+      <c r="Q48" s="15"/>
+      <c r="R48" s="15"/>
     </row>
     <row r="49" s="1" customFormat="1" spans="1:18">
-      <c r="A49" s="14">
+      <c r="A49" s="13">
         <v>54</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="16" t="s">
         <v>81</v>
       </c>
       <c r="C49" s="10"/>
-      <c r="D49" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" s="16" t="s">
+      <c r="D49" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E49" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F49" s="12" t="s">
@@ -3563,31 +3578,31 @@
       <c r="H49" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I49" s="16" t="s">
+      <c r="I49" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J49" s="26"/>
-      <c r="K49" s="27"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="26"/>
       <c r="L49" s="10"/>
       <c r="M49" s="10"/>
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
-      <c r="P49" s="16"/>
-      <c r="Q49" s="16"/>
-      <c r="R49" s="16"/>
+      <c r="P49" s="15"/>
+      <c r="Q49" s="15"/>
+      <c r="R49" s="15"/>
     </row>
     <row r="50" s="1" customFormat="1" spans="1:18">
-      <c r="A50" s="14">
+      <c r="A50" s="13">
         <v>55</v>
       </c>
-      <c r="B50" s="17" t="s">
+      <c r="B50" s="16" t="s">
         <v>82</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" s="16" t="s">
+      <c r="D50" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E50" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F50" s="12" t="s">
@@ -3599,24 +3614,24 @@
       <c r="H50" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I50" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J50" s="26"/>
-      <c r="K50" s="27"/>
+      <c r="I50" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J50" s="25"/>
+      <c r="K50" s="26"/>
       <c r="L50" s="10"/>
       <c r="M50" s="10"/>
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
-      <c r="P50" s="16"/>
-      <c r="Q50" s="16"/>
-      <c r="R50" s="16"/>
+      <c r="P50" s="15"/>
+      <c r="Q50" s="15"/>
+      <c r="R50" s="15"/>
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="3">
         <v>56</v>
       </c>
-      <c r="B51" s="18" t="s">
+      <c r="B51" s="17" t="s">
         <v>83</v>
       </c>
       <c r="C51" s="10"/>
@@ -3638,8 +3653,8 @@
       <c r="I51" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J51" s="24"/>
-      <c r="K51" s="25"/>
+      <c r="J51" s="23"/>
+      <c r="K51" s="24"/>
       <c r="L51" s="12"/>
       <c r="M51" s="12"/>
       <c r="N51" s="12"/>
@@ -3649,17 +3664,17 @@
       <c r="R51" s="11"/>
     </row>
     <row r="52" s="1" customFormat="1" spans="1:18">
-      <c r="A52" s="14">
+      <c r="A52" s="13">
         <v>57</v>
       </c>
-      <c r="B52" s="19" t="s">
+      <c r="B52" s="18" t="s">
         <v>84</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E52" s="16" t="s">
+      <c r="D52" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E52" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F52" s="12" t="s">
@@ -3671,31 +3686,31 @@
       <c r="H52" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I52" s="16" t="s">
+      <c r="I52" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J52" s="26"/>
-      <c r="K52" s="27"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="26"/>
       <c r="L52" s="10"/>
       <c r="M52" s="10"/>
       <c r="N52" s="10"/>
       <c r="O52" s="10"/>
-      <c r="P52" s="16"/>
-      <c r="Q52" s="16"/>
-      <c r="R52" s="16"/>
+      <c r="P52" s="15"/>
+      <c r="Q52" s="15"/>
+      <c r="R52" s="15"/>
     </row>
     <row r="53" s="1" customFormat="1" spans="1:18">
-      <c r="A53" s="14">
+      <c r="A53" s="13">
         <v>58</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="18" t="s">
         <v>85</v>
       </c>
       <c r="C53" s="10"/>
-      <c r="D53" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E53" s="16" t="s">
+      <c r="D53" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E53" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F53" s="12" t="s">
@@ -3707,31 +3722,31 @@
       <c r="H53" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I53" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J53" s="26"/>
-      <c r="K53" s="27"/>
+      <c r="I53" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J53" s="25"/>
+      <c r="K53" s="26"/>
       <c r="L53" s="10"/>
       <c r="M53" s="10"/>
       <c r="N53" s="10"/>
       <c r="O53" s="10"/>
-      <c r="P53" s="16"/>
-      <c r="Q53" s="16"/>
-      <c r="R53" s="16"/>
+      <c r="P53" s="15"/>
+      <c r="Q53" s="15"/>
+      <c r="R53" s="15"/>
     </row>
     <row r="54" s="1" customFormat="1" spans="1:18">
-      <c r="A54" s="14">
+      <c r="A54" s="13">
         <v>59</v>
       </c>
-      <c r="B54" s="19" t="s">
+      <c r="B54" s="18" t="s">
         <v>86</v>
       </c>
       <c r="C54" s="10"/>
-      <c r="D54" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54" s="16" t="s">
+      <c r="D54" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E54" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F54" s="12" t="s">
@@ -3743,31 +3758,31 @@
       <c r="H54" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I54" s="16" t="s">
+      <c r="I54" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J54" s="26"/>
-      <c r="K54" s="27"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="26"/>
       <c r="L54" s="10"/>
       <c r="M54" s="10"/>
       <c r="N54" s="10"/>
       <c r="O54" s="10"/>
-      <c r="P54" s="16"/>
-      <c r="Q54" s="16"/>
-      <c r="R54" s="16"/>
+      <c r="P54" s="15"/>
+      <c r="Q54" s="15"/>
+      <c r="R54" s="15"/>
     </row>
     <row r="55" s="1" customFormat="1" spans="1:18">
-      <c r="A55" s="14">
+      <c r="A55" s="13">
         <v>62</v>
       </c>
-      <c r="B55" s="19" t="s">
+      <c r="B55" s="18" t="s">
         <v>87</v>
       </c>
       <c r="C55" s="10"/>
-      <c r="D55" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E55" s="16" t="s">
+      <c r="D55" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E55" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F55" s="12" t="s">
@@ -3779,31 +3794,31 @@
       <c r="H55" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I55" s="16" t="s">
+      <c r="I55" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="J55" s="26"/>
-      <c r="K55" s="27"/>
+      <c r="J55" s="25"/>
+      <c r="K55" s="26"/>
       <c r="L55" s="10"/>
       <c r="M55" s="10"/>
       <c r="N55" s="10"/>
       <c r="O55" s="10"/>
-      <c r="P55" s="16"/>
-      <c r="Q55" s="16"/>
-      <c r="R55" s="16"/>
+      <c r="P55" s="15"/>
+      <c r="Q55" s="15"/>
+      <c r="R55" s="15"/>
     </row>
     <row r="56" s="1" customFormat="1" spans="1:18">
-      <c r="A56" s="14">
+      <c r="A56" s="13">
         <v>63</v>
       </c>
-      <c r="B56" s="19" t="s">
+      <c r="B56" s="18" t="s">
         <v>88</v>
       </c>
       <c r="C56" s="10"/>
-      <c r="D56" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" s="16" t="s">
+      <c r="D56" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E56" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F56" s="12" t="s">
@@ -3815,31 +3830,31 @@
       <c r="H56" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I56" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J56" s="26"/>
-      <c r="K56" s="27"/>
+      <c r="I56" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J56" s="25"/>
+      <c r="K56" s="26"/>
       <c r="L56" s="10"/>
       <c r="M56" s="10"/>
       <c r="N56" s="10"/>
       <c r="O56" s="10"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="16"/>
-      <c r="R56" s="16"/>
+      <c r="P56" s="15"/>
+      <c r="Q56" s="15"/>
+      <c r="R56" s="15"/>
     </row>
     <row r="57" spans="1:18">
       <c r="A57" s="3">
         <v>64</v>
       </c>
-      <c r="B57" s="19" t="s">
+      <c r="B57" s="18" t="s">
         <v>89</v>
       </c>
       <c r="C57" s="12"/>
       <c r="D57" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E57" s="16" t="s">
+      <c r="E57" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F57" s="12" t="s">
@@ -3854,8 +3869,8 @@
       <c r="I57" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J57" s="24"/>
-      <c r="K57" s="25"/>
+      <c r="J57" s="23"/>
+      <c r="K57" s="24"/>
       <c r="L57" s="12"/>
       <c r="M57" s="12"/>
       <c r="N57" s="12"/>
@@ -3868,14 +3883,14 @@
       <c r="A58" s="3">
         <v>65</v>
       </c>
-      <c r="B58" s="19" t="s">
+      <c r="B58" s="18" t="s">
         <v>90</v>
       </c>
       <c r="C58" s="12"/>
       <c r="D58" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E58" s="16" t="s">
+      <c r="E58" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F58" s="12" t="s">
@@ -3890,8 +3905,8 @@
       <c r="I58" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J58" s="24"/>
-      <c r="K58" s="25"/>
+      <c r="J58" s="23"/>
+      <c r="K58" s="24"/>
       <c r="L58" s="12"/>
       <c r="M58" s="12"/>
       <c r="N58" s="12"/>
@@ -3904,14 +3919,14 @@
       <c r="A59" s="3">
         <v>66</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="18" t="s">
         <v>91</v>
       </c>
       <c r="C59" s="12"/>
       <c r="D59" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E59" s="16" t="s">
+      <c r="E59" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F59" s="12" t="s">
@@ -3926,8 +3941,8 @@
       <c r="I59" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J59" s="24"/>
-      <c r="K59" s="25"/>
+      <c r="J59" s="23"/>
+      <c r="K59" s="24"/>
       <c r="L59" s="12"/>
       <c r="M59" s="12"/>
       <c r="N59" s="12"/>
@@ -3937,17 +3952,17 @@
       <c r="R59" s="11"/>
     </row>
     <row r="60" s="1" customFormat="1" spans="1:18">
-      <c r="A60" s="14">
+      <c r="A60" s="13">
         <v>67</v>
       </c>
-      <c r="B60" s="19" t="s">
+      <c r="B60" s="18" t="s">
         <v>92</v>
       </c>
       <c r="C60" s="10"/>
-      <c r="D60" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E60" s="16" t="s">
+      <c r="D60" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E60" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F60" s="12" t="s">
@@ -3959,31 +3974,31 @@
       <c r="H60" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I60" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J60" s="26"/>
-      <c r="K60" s="27"/>
+      <c r="I60" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J60" s="25"/>
+      <c r="K60" s="26"/>
       <c r="L60" s="10"/>
       <c r="M60" s="10"/>
       <c r="N60" s="10"/>
       <c r="O60" s="10"/>
-      <c r="P60" s="16"/>
-      <c r="Q60" s="16"/>
-      <c r="R60" s="16"/>
+      <c r="P60" s="15"/>
+      <c r="Q60" s="15"/>
+      <c r="R60" s="15"/>
     </row>
     <row r="61" spans="1:18">
       <c r="A61" s="3">
         <v>68</v>
       </c>
-      <c r="B61" s="19" t="s">
+      <c r="B61" s="18" t="s">
         <v>93</v>
       </c>
       <c r="C61" s="12"/>
       <c r="D61" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E61" s="16" t="s">
+      <c r="E61" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F61" s="12" t="s">
@@ -3998,8 +4013,8 @@
       <c r="I61" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J61" s="24"/>
-      <c r="K61" s="25"/>
+      <c r="J61" s="23"/>
+      <c r="K61" s="24"/>
       <c r="L61" s="12"/>
       <c r="M61" s="12"/>
       <c r="N61" s="12"/>
@@ -4009,17 +4024,17 @@
       <c r="R61" s="11"/>
     </row>
     <row r="62" s="1" customFormat="1" spans="1:18">
-      <c r="A62" s="14">
+      <c r="A62" s="13">
         <v>69</v>
       </c>
-      <c r="B62" s="19" t="s">
+      <c r="B62" s="18" t="s">
         <v>94</v>
       </c>
       <c r="C62" s="10"/>
-      <c r="D62" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E62" s="16" t="s">
+      <c r="D62" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F62" s="12" t="s">
@@ -4031,31 +4046,31 @@
       <c r="H62" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I62" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J62" s="26"/>
-      <c r="K62" s="27"/>
+      <c r="I62" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J62" s="25"/>
+      <c r="K62" s="26"/>
       <c r="L62" s="10"/>
       <c r="M62" s="10"/>
       <c r="N62" s="10"/>
       <c r="O62" s="10"/>
-      <c r="P62" s="16"/>
-      <c r="Q62" s="16"/>
-      <c r="R62" s="16"/>
+      <c r="P62" s="15"/>
+      <c r="Q62" s="15"/>
+      <c r="R62" s="15"/>
     </row>
     <row r="63" spans="1:18">
       <c r="A63" s="3">
         <v>70</v>
       </c>
-      <c r="B63" s="19" t="s">
+      <c r="B63" s="18" t="s">
         <v>95</v>
       </c>
       <c r="C63" s="12"/>
       <c r="D63" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E63" s="16" t="s">
+      <c r="E63" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F63" s="12" t="s">
@@ -4070,8 +4085,8 @@
       <c r="I63" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J63" s="24"/>
-      <c r="K63" s="25"/>
+      <c r="J63" s="23"/>
+      <c r="K63" s="24"/>
       <c r="L63" s="12"/>
       <c r="M63" s="12"/>
       <c r="N63" s="12"/>
@@ -4081,17 +4096,17 @@
       <c r="R63" s="11"/>
     </row>
     <row r="64" s="1" customFormat="1" spans="1:18">
-      <c r="A64" s="14">
+      <c r="A64" s="13">
         <v>71</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B64" s="18" t="s">
         <v>96</v>
       </c>
       <c r="C64" s="10"/>
-      <c r="D64" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E64" s="16" t="s">
+      <c r="D64" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F64" s="12" t="s">
@@ -4103,31 +4118,31 @@
       <c r="H64" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I64" s="16" t="s">
+      <c r="I64" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J64" s="26"/>
-      <c r="K64" s="27"/>
+      <c r="J64" s="25"/>
+      <c r="K64" s="26"/>
       <c r="L64" s="10"/>
       <c r="M64" s="10"/>
       <c r="N64" s="10"/>
       <c r="O64" s="10"/>
-      <c r="P64" s="16"/>
-      <c r="Q64" s="16"/>
-      <c r="R64" s="16"/>
+      <c r="P64" s="15"/>
+      <c r="Q64" s="15"/>
+      <c r="R64" s="15"/>
     </row>
     <row r="65" s="1" customFormat="1" spans="1:18">
-      <c r="A65" s="14">
+      <c r="A65" s="13">
         <v>72</v>
       </c>
-      <c r="B65" s="19" t="s">
+      <c r="B65" s="18" t="s">
         <v>97</v>
       </c>
       <c r="C65" s="10"/>
-      <c r="D65" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E65" s="16" t="s">
+      <c r="D65" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E65" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F65" s="12" t="s">
@@ -4139,31 +4154,31 @@
       <c r="H65" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I65" s="16" t="s">
+      <c r="I65" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="J65" s="26"/>
-      <c r="K65" s="27"/>
+      <c r="J65" s="25"/>
+      <c r="K65" s="26"/>
       <c r="L65" s="10"/>
       <c r="M65" s="10"/>
       <c r="N65" s="10"/>
       <c r="O65" s="10"/>
-      <c r="P65" s="16"/>
-      <c r="Q65" s="16"/>
-      <c r="R65" s="16"/>
+      <c r="P65" s="15"/>
+      <c r="Q65" s="15"/>
+      <c r="R65" s="15"/>
     </row>
     <row r="66" spans="1:18">
       <c r="A66" s="3">
         <v>73</v>
       </c>
-      <c r="B66" s="19" t="s">
+      <c r="B66" s="18" t="s">
         <v>98</v>
       </c>
       <c r="C66" s="12"/>
       <c r="D66" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E66" s="16" t="s">
+      <c r="E66" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F66" s="12" t="s">
@@ -4178,8 +4193,8 @@
       <c r="I66" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J66" s="24"/>
-      <c r="K66" s="25"/>
+      <c r="J66" s="23"/>
+      <c r="K66" s="24"/>
       <c r="L66" s="12"/>
       <c r="M66" s="12"/>
       <c r="N66" s="12"/>
@@ -4189,17 +4204,17 @@
       <c r="R66" s="11"/>
     </row>
     <row r="67" s="1" customFormat="1" spans="1:18">
-      <c r="A67" s="14">
+      <c r="A67" s="13">
         <v>74</v>
       </c>
-      <c r="B67" s="28" t="s">
+      <c r="B67" s="27" t="s">
         <v>99</v>
       </c>
       <c r="C67" s="10"/>
-      <c r="D67" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E67" s="16" t="s">
+      <c r="D67" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E67" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F67" s="12" t="s">
@@ -4211,31 +4226,31 @@
       <c r="H67" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I67" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J67" s="26"/>
-      <c r="K67" s="27"/>
+      <c r="I67" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J67" s="25"/>
+      <c r="K67" s="26"/>
       <c r="L67" s="10"/>
       <c r="M67" s="10"/>
       <c r="N67" s="10"/>
       <c r="O67" s="10"/>
-      <c r="P67" s="16"/>
-      <c r="Q67" s="16"/>
-      <c r="R67" s="16"/>
+      <c r="P67" s="15"/>
+      <c r="Q67" s="15"/>
+      <c r="R67" s="15"/>
     </row>
     <row r="68" s="1" customFormat="1" spans="1:18">
-      <c r="A68" s="14">
+      <c r="A68" s="13">
         <v>75</v>
       </c>
-      <c r="B68" s="28" t="s">
+      <c r="B68" s="27" t="s">
         <v>100</v>
       </c>
       <c r="C68" s="10"/>
-      <c r="D68" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E68" s="16" t="s">
+      <c r="D68" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E68" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F68" s="12" t="s">
@@ -4247,31 +4262,31 @@
       <c r="H68" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I68" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J68" s="26"/>
-      <c r="K68" s="27"/>
+      <c r="I68" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J68" s="25"/>
+      <c r="K68" s="26"/>
       <c r="L68" s="10"/>
       <c r="M68" s="10"/>
       <c r="N68" s="10"/>
       <c r="O68" s="10"/>
-      <c r="P68" s="16"/>
-      <c r="Q68" s="16"/>
-      <c r="R68" s="16"/>
+      <c r="P68" s="15"/>
+      <c r="Q68" s="15"/>
+      <c r="R68" s="15"/>
     </row>
     <row r="69" spans="1:18">
       <c r="A69" s="3">
         <v>76</v>
       </c>
-      <c r="B69" s="28" t="s">
+      <c r="B69" s="27" t="s">
         <v>101</v>
       </c>
       <c r="C69" s="12"/>
       <c r="D69" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E69" s="16" t="s">
+      <c r="E69" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F69" s="12" t="s">
@@ -4286,8 +4301,8 @@
       <c r="I69" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J69" s="24"/>
-      <c r="K69" s="25"/>
+      <c r="J69" s="23"/>
+      <c r="K69" s="24"/>
       <c r="L69" s="12"/>
       <c r="M69" s="12"/>
       <c r="N69" s="12"/>
@@ -4300,14 +4315,14 @@
       <c r="A70" s="3">
         <v>77</v>
       </c>
-      <c r="B70" s="28" t="s">
+      <c r="B70" s="27" t="s">
         <v>102</v>
       </c>
       <c r="C70" s="12"/>
       <c r="D70" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E70" s="16" t="s">
+      <c r="E70" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F70" s="12" t="s">
@@ -4322,8 +4337,8 @@
       <c r="I70" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J70" s="24"/>
-      <c r="K70" s="25"/>
+      <c r="J70" s="23"/>
+      <c r="K70" s="24"/>
       <c r="L70" s="12"/>
       <c r="M70" s="12"/>
       <c r="N70" s="12"/>
@@ -4333,17 +4348,17 @@
       <c r="R70" s="11"/>
     </row>
     <row r="71" s="1" customFormat="1" ht="12" customHeight="1" spans="1:18">
-      <c r="A71" s="14">
+      <c r="A71" s="13">
         <v>78</v>
       </c>
-      <c r="B71" s="28" t="s">
+      <c r="B71" s="27" t="s">
         <v>103</v>
       </c>
       <c r="C71" s="10"/>
-      <c r="D71" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E71" s="16" t="s">
+      <c r="D71" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E71" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F71" s="12" t="s">
@@ -4355,31 +4370,31 @@
       <c r="H71" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I71" s="16" t="s">
+      <c r="I71" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="J71" s="26"/>
-      <c r="K71" s="27"/>
+      <c r="J71" s="25"/>
+      <c r="K71" s="26"/>
       <c r="L71" s="10"/>
       <c r="M71" s="10"/>
       <c r="N71" s="10"/>
       <c r="O71" s="10"/>
-      <c r="P71" s="16"/>
-      <c r="Q71" s="16"/>
-      <c r="R71" s="16"/>
+      <c r="P71" s="15"/>
+      <c r="Q71" s="15"/>
+      <c r="R71" s="15"/>
     </row>
     <row r="72" s="1" customFormat="1" spans="1:18">
-      <c r="A72" s="14">
+      <c r="A72" s="13">
         <v>79</v>
       </c>
-      <c r="B72" s="28" t="s">
+      <c r="B72" s="27" t="s">
         <v>104</v>
       </c>
       <c r="C72" s="10"/>
-      <c r="D72" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E72" s="16" t="s">
+      <c r="D72" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E72" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F72" s="12" t="s">
@@ -4391,31 +4406,31 @@
       <c r="H72" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I72" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J72" s="26"/>
-      <c r="K72" s="27"/>
+      <c r="I72" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J72" s="25"/>
+      <c r="K72" s="26"/>
       <c r="L72" s="10"/>
       <c r="M72" s="10"/>
       <c r="N72" s="10"/>
       <c r="O72" s="10"/>
-      <c r="P72" s="16"/>
-      <c r="Q72" s="16"/>
-      <c r="R72" s="16"/>
+      <c r="P72" s="15"/>
+      <c r="Q72" s="15"/>
+      <c r="R72" s="15"/>
     </row>
     <row r="73" s="1" customFormat="1" spans="1:18">
-      <c r="A73" s="14">
+      <c r="A73" s="13">
         <v>80</v>
       </c>
-      <c r="B73" s="28" t="s">
+      <c r="B73" s="27" t="s">
         <v>105</v>
       </c>
       <c r="C73" s="10"/>
-      <c r="D73" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E73" s="16" t="s">
+      <c r="D73" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E73" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F73" s="12" t="s">
@@ -4427,31 +4442,31 @@
       <c r="H73" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I73" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J73" s="26"/>
-      <c r="K73" s="27"/>
+      <c r="I73" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" s="25"/>
+      <c r="K73" s="26"/>
       <c r="L73" s="10"/>
       <c r="M73" s="10"/>
       <c r="N73" s="10"/>
       <c r="O73" s="10"/>
-      <c r="P73" s="16"/>
-      <c r="Q73" s="16"/>
-      <c r="R73" s="16"/>
+      <c r="P73" s="15"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="15"/>
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="3">
         <v>81</v>
       </c>
-      <c r="B74" s="28" t="s">
+      <c r="B74" s="27" t="s">
         <v>106</v>
       </c>
       <c r="C74" s="12"/>
       <c r="D74" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="E74" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F74" s="12" t="s">
@@ -4466,8 +4481,8 @@
       <c r="I74" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="24"/>
-      <c r="K74" s="25"/>
+      <c r="J74" s="23"/>
+      <c r="K74" s="24"/>
       <c r="L74" s="12"/>
       <c r="M74" s="12"/>
       <c r="N74" s="12"/>
@@ -4477,17 +4492,17 @@
       <c r="R74" s="11"/>
     </row>
     <row r="75" s="1" customFormat="1" spans="1:18">
-      <c r="A75" s="14">
+      <c r="A75" s="13">
         <v>82</v>
       </c>
-      <c r="B75" s="28" t="s">
+      <c r="B75" s="27" t="s">
         <v>107</v>
       </c>
       <c r="C75" s="10"/>
-      <c r="D75" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E75" s="16" t="s">
+      <c r="D75" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E75" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F75" s="12" t="s">
@@ -4499,31 +4514,31 @@
       <c r="H75" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I75" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J75" s="26"/>
-      <c r="K75" s="27"/>
+      <c r="I75" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J75" s="25"/>
+      <c r="K75" s="26"/>
       <c r="L75" s="10"/>
       <c r="M75" s="10"/>
       <c r="N75" s="10"/>
       <c r="O75" s="10"/>
-      <c r="P75" s="16"/>
-      <c r="Q75" s="16"/>
-      <c r="R75" s="16"/>
+      <c r="P75" s="15"/>
+      <c r="Q75" s="15"/>
+      <c r="R75" s="15"/>
     </row>
     <row r="76" s="1" customFormat="1" spans="1:18">
-      <c r="A76" s="14">
+      <c r="A76" s="13">
         <v>83</v>
       </c>
-      <c r="B76" s="28" t="s">
+      <c r="B76" s="27" t="s">
         <v>108</v>
       </c>
       <c r="C76" s="10"/>
-      <c r="D76" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E76" s="16" t="s">
+      <c r="D76" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E76" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F76" s="12" t="s">
@@ -4535,31 +4550,31 @@
       <c r="H76" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I76" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J76" s="26"/>
-      <c r="K76" s="27"/>
+      <c r="I76" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J76" s="25"/>
+      <c r="K76" s="26"/>
       <c r="L76" s="10"/>
       <c r="M76" s="10"/>
       <c r="N76" s="10"/>
       <c r="O76" s="10"/>
-      <c r="P76" s="16"/>
-      <c r="Q76" s="16"/>
-      <c r="R76" s="16"/>
+      <c r="P76" s="15"/>
+      <c r="Q76" s="15"/>
+      <c r="R76" s="15"/>
     </row>
     <row r="77" s="1" customFormat="1" spans="1:18">
-      <c r="A77" s="14">
+      <c r="A77" s="13">
         <v>84</v>
       </c>
-      <c r="B77" s="28" t="s">
+      <c r="B77" s="27" t="s">
         <v>109</v>
       </c>
       <c r="C77" s="10"/>
-      <c r="D77" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E77" s="16" t="s">
+      <c r="D77" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E77" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F77" s="12" t="s">
@@ -4571,31 +4586,31 @@
       <c r="H77" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I77" s="16" t="s">
+      <c r="I77" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J77" s="26"/>
-      <c r="K77" s="27"/>
+      <c r="J77" s="25"/>
+      <c r="K77" s="26"/>
       <c r="L77" s="10"/>
       <c r="M77" s="10"/>
       <c r="N77" s="10"/>
       <c r="O77" s="10"/>
-      <c r="P77" s="16"/>
-      <c r="Q77" s="16"/>
-      <c r="R77" s="16"/>
+      <c r="P77" s="15"/>
+      <c r="Q77" s="15"/>
+      <c r="R77" s="15"/>
     </row>
     <row r="78" s="1" customFormat="1" spans="1:18">
-      <c r="A78" s="14">
+      <c r="A78" s="13">
         <v>85</v>
       </c>
-      <c r="B78" s="28" t="s">
+      <c r="B78" s="27" t="s">
         <v>110</v>
       </c>
       <c r="C78" s="10"/>
-      <c r="D78" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E78" s="16" t="s">
+      <c r="D78" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E78" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F78" s="12" t="s">
@@ -4607,31 +4622,31 @@
       <c r="H78" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I78" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J78" s="26"/>
-      <c r="K78" s="27"/>
+      <c r="I78" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J78" s="25"/>
+      <c r="K78" s="26"/>
       <c r="L78" s="10"/>
       <c r="M78" s="10"/>
       <c r="N78" s="10"/>
       <c r="O78" s="10"/>
-      <c r="P78" s="16"/>
-      <c r="Q78" s="16"/>
-      <c r="R78" s="16"/>
+      <c r="P78" s="15"/>
+      <c r="Q78" s="15"/>
+      <c r="R78" s="15"/>
     </row>
     <row r="79" s="1" customFormat="1" spans="1:18">
-      <c r="A79" s="14">
+      <c r="A79" s="13">
         <v>88</v>
       </c>
-      <c r="B79" s="28" t="s">
+      <c r="B79" s="27" t="s">
         <v>111</v>
       </c>
       <c r="C79" s="10"/>
-      <c r="D79" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E79" s="16" t="s">
+      <c r="D79" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E79" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F79" s="12" t="s">
@@ -4643,31 +4658,31 @@
       <c r="H79" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I79" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J79" s="26"/>
-      <c r="K79" s="27"/>
+      <c r="I79" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J79" s="25"/>
+      <c r="K79" s="26"/>
       <c r="L79" s="10"/>
       <c r="M79" s="10"/>
       <c r="N79" s="10"/>
       <c r="O79" s="10"/>
-      <c r="P79" s="16"/>
-      <c r="Q79" s="16"/>
-      <c r="R79" s="16"/>
+      <c r="P79" s="15"/>
+      <c r="Q79" s="15"/>
+      <c r="R79" s="15"/>
     </row>
     <row r="80" s="1" customFormat="1" spans="1:18">
-      <c r="A80" s="14">
+      <c r="A80" s="13">
         <v>89</v>
       </c>
-      <c r="B80" s="28" t="s">
+      <c r="B80" s="27" t="s">
         <v>112</v>
       </c>
       <c r="C80" s="10"/>
-      <c r="D80" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E80" s="16" t="s">
+      <c r="D80" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="E80" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F80" s="12" t="s">
@@ -4679,31 +4694,31 @@
       <c r="H80" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I80" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="J80" s="26"/>
-      <c r="K80" s="27"/>
+      <c r="I80" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J80" s="25"/>
+      <c r="K80" s="26"/>
       <c r="L80" s="10"/>
       <c r="M80" s="10"/>
       <c r="N80" s="10"/>
       <c r="O80" s="10"/>
-      <c r="P80" s="16"/>
-      <c r="Q80" s="16"/>
-      <c r="R80" s="16"/>
+      <c r="P80" s="15"/>
+      <c r="Q80" s="15"/>
+      <c r="R80" s="15"/>
     </row>
     <row r="81" spans="1:18">
       <c r="A81" s="3">
         <v>90</v>
       </c>
-      <c r="B81" s="28" t="s">
+      <c r="B81" s="27" t="s">
         <v>113</v>
       </c>
       <c r="C81" s="12"/>
       <c r="D81" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E81" s="16" t="s">
+      <c r="E81" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F81" s="12" t="s">
@@ -4718,8 +4733,8 @@
       <c r="I81" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J81" s="24"/>
-      <c r="K81" s="25"/>
+      <c r="J81" s="23"/>
+      <c r="K81" s="24"/>
       <c r="L81" s="12"/>
       <c r="M81" s="12"/>
       <c r="N81" s="12"/>
@@ -4732,14 +4747,14 @@
       <c r="A82" s="3">
         <v>91</v>
       </c>
-      <c r="B82" s="28" t="s">
+      <c r="B82" s="27" t="s">
         <v>114</v>
       </c>
       <c r="C82" s="12"/>
       <c r="D82" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E82" s="16" t="s">
+      <c r="E82" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F82" s="12" t="s">
@@ -4754,8 +4769,8 @@
       <c r="I82" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J82" s="24"/>
-      <c r="K82" s="25"/>
+      <c r="J82" s="23"/>
+      <c r="K82" s="24"/>
       <c r="L82" s="12"/>
       <c r="M82" s="12"/>
       <c r="N82" s="12"/>
@@ -4768,14 +4783,14 @@
       <c r="A83" s="3">
         <v>92</v>
       </c>
-      <c r="B83" s="29" t="s">
+      <c r="B83" s="28" t="s">
         <v>115</v>
       </c>
       <c r="C83" s="12"/>
       <c r="D83" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E83" s="16" t="s">
+      <c r="E83" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F83" s="12" t="s">
@@ -4790,8 +4805,8 @@
       <c r="I83" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J83" s="24"/>
-      <c r="K83" s="25"/>
+      <c r="J83" s="23"/>
+      <c r="K83" s="24"/>
       <c r="L83" s="12"/>
       <c r="M83" s="12"/>
       <c r="N83" s="12"/>
@@ -4804,14 +4819,14 @@
       <c r="A84" s="3">
         <v>93</v>
       </c>
-      <c r="B84" s="29" t="s">
+      <c r="B84" s="28" t="s">
         <v>116</v>
       </c>
       <c r="C84" s="12"/>
       <c r="D84" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E84" s="16" t="s">
+      <c r="E84" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F84" s="12" t="s">
@@ -4826,8 +4841,8 @@
       <c r="I84" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J84" s="24"/>
-      <c r="K84" s="25"/>
+      <c r="J84" s="23"/>
+      <c r="K84" s="24"/>
       <c r="L84" s="12"/>
       <c r="M84" s="12"/>
       <c r="N84" s="12"/>
@@ -4840,14 +4855,14 @@
       <c r="A85" s="3">
         <v>94</v>
       </c>
-      <c r="B85" s="29" t="s">
+      <c r="B85" s="28" t="s">
         <v>117</v>
       </c>
       <c r="C85" s="12"/>
       <c r="D85" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E85" s="16" t="s">
+      <c r="E85" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F85" s="12" t="s">
@@ -4862,8 +4877,8 @@
       <c r="I85" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J85" s="24"/>
-      <c r="K85" s="25"/>
+      <c r="J85" s="23"/>
+      <c r="K85" s="24"/>
       <c r="L85" s="12"/>
       <c r="M85" s="12"/>
       <c r="N85" s="12"/>
@@ -4876,14 +4891,14 @@
       <c r="A86" s="3">
         <v>95</v>
       </c>
-      <c r="B86" s="29" t="s">
+      <c r="B86" s="28" t="s">
         <v>118</v>
       </c>
       <c r="C86" s="12"/>
       <c r="D86" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E86" s="16" t="s">
+      <c r="E86" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F86" s="12" t="s">
@@ -4898,8 +4913,8 @@
       <c r="I86" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J86" s="24"/>
-      <c r="K86" s="25"/>
+      <c r="J86" s="23"/>
+      <c r="K86" s="24"/>
       <c r="L86" s="12"/>
       <c r="M86" s="12"/>
       <c r="N86" s="12"/>
@@ -4912,14 +4927,14 @@
       <c r="A87" s="3">
         <v>96</v>
       </c>
-      <c r="B87" s="29" t="s">
+      <c r="B87" s="28" t="s">
         <v>119</v>
       </c>
       <c r="C87" s="12"/>
       <c r="D87" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="16" t="s">
+      <c r="E87" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F87" s="12" t="s">
@@ -4934,8 +4949,8 @@
       <c r="I87" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J87" s="24"/>
-      <c r="K87" s="25"/>
+      <c r="J87" s="23"/>
+      <c r="K87" s="24"/>
       <c r="L87" s="12"/>
       <c r="M87" s="12"/>
       <c r="N87" s="12"/>
@@ -4948,14 +4963,14 @@
       <c r="A88" s="3">
         <v>97</v>
       </c>
-      <c r="B88" s="29" t="s">
+      <c r="B88" s="28" t="s">
         <v>120</v>
       </c>
       <c r="C88" s="12"/>
       <c r="D88" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E88" s="16" t="s">
+      <c r="E88" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F88" s="12" t="s">
@@ -4970,8 +4985,8 @@
       <c r="I88" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J88" s="24"/>
-      <c r="K88" s="25"/>
+      <c r="J88" s="23"/>
+      <c r="K88" s="24"/>
       <c r="L88" s="12"/>
       <c r="M88" s="12"/>
       <c r="N88" s="12"/>
@@ -4984,21 +4999,23 @@
       <c r="A89" s="3">
         <v>98</v>
       </c>
-      <c r="B89" s="29" t="s">
+      <c r="B89" s="28" t="s">
         <v>121</v>
       </c>
-      <c r="C89" s="12"/>
+      <c r="C89" s="29" t="s">
+        <v>122</v>
+      </c>
       <c r="D89" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E89" s="16" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="E89" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="F89" s="12" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="G89" s="12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="H89" s="11" t="s">
         <v>17</v>
@@ -5006,8 +5023,8 @@
       <c r="I89" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J89" s="24"/>
-      <c r="K89" s="25"/>
+      <c r="J89" s="23"/>
+      <c r="K89" s="24"/>
       <c r="L89" s="12"/>
       <c r="M89" s="12"/>
       <c r="N89" s="12"/>
@@ -5020,30 +5037,32 @@
       <c r="A90" s="3">
         <v>99</v>
       </c>
-      <c r="B90" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C90" s="12"/>
+      <c r="B90" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C90" s="29" t="s">
+        <v>124</v>
+      </c>
       <c r="D90" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E90" s="16" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="E90" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="F90" s="12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G90" s="12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="H90" s="11" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="I90" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J90" s="24"/>
-      <c r="K90" s="25"/>
+      <c r="J90" s="23"/>
+      <c r="K90" s="24"/>
       <c r="L90" s="12"/>
       <c r="M90" s="12"/>
       <c r="N90" s="12"/>
@@ -5056,30 +5075,32 @@
       <c r="A91" s="3">
         <v>100</v>
       </c>
-      <c r="B91" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="C91" s="12"/>
+      <c r="B91" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="C91" s="29" t="s">
+        <v>127</v>
+      </c>
       <c r="D91" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E91" s="16" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="E91" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="F91" s="12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G91" s="12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="H91" s="11" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="I91" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J91" s="24"/>
-      <c r="K91" s="25"/>
+      <c r="J91" s="23"/>
+      <c r="K91" s="24"/>
       <c r="L91" s="12"/>
       <c r="M91" s="12"/>
       <c r="N91" s="12"/>
@@ -5092,29 +5113,31 @@
       <c r="A92" s="3">
         <v>101</v>
       </c>
-      <c r="B92" s="29" t="s">
-        <v>124</v>
-      </c>
-      <c r="C92" s="12"/>
+      <c r="B92" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="C92" s="29" t="s">
+        <v>129</v>
+      </c>
       <c r="D92" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E92" s="16" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="E92" s="15" t="s">
+        <v>33</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="G92" s="12" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="H92" s="11" t="s">
-        <v>17</v>
+        <v>125</v>
       </c>
       <c r="I92" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J92" s="24"/>
+      <c r="J92" s="23"/>
       <c r="K92" s="12"/>
       <c r="L92" s="12"/>
       <c r="M92" s="12"/>
@@ -5128,14 +5151,14 @@
       <c r="A93" s="3">
         <v>102</v>
       </c>
-      <c r="B93" s="29" t="s">
-        <v>125</v>
+      <c r="B93" s="28" t="s">
+        <v>130</v>
       </c>
       <c r="C93" s="12"/>
       <c r="D93" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E93" s="16" t="s">
+      <c r="E93" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F93" s="12" t="s">
@@ -5150,7 +5173,7 @@
       <c r="I93" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J93" s="24"/>
+      <c r="J93" s="23"/>
       <c r="K93" s="12"/>
       <c r="L93" s="12"/>
       <c r="M93" s="12"/>
@@ -5164,14 +5187,14 @@
       <c r="A94" s="3">
         <v>103</v>
       </c>
-      <c r="B94" s="29" t="s">
-        <v>126</v>
+      <c r="B94" s="28" t="s">
+        <v>131</v>
       </c>
       <c r="C94" s="12"/>
       <c r="D94" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E94" s="16" t="s">
+      <c r="E94" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F94" s="12" t="s">
@@ -5186,7 +5209,7 @@
       <c r="I94" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J94" s="24"/>
+      <c r="J94" s="23"/>
       <c r="K94" s="12"/>
       <c r="L94" s="12"/>
       <c r="M94" s="12"/>
@@ -5200,14 +5223,14 @@
       <c r="A95" s="3">
         <v>104</v>
       </c>
-      <c r="B95" s="29" t="s">
-        <v>127</v>
+      <c r="B95" s="28" t="s">
+        <v>132</v>
       </c>
       <c r="C95" s="12"/>
       <c r="D95" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E95" s="16" t="s">
+      <c r="E95" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F95" s="12" t="s">
@@ -5222,7 +5245,7 @@
       <c r="I95" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J95" s="24"/>
+      <c r="J95" s="23"/>
       <c r="K95" s="12"/>
       <c r="L95" s="12"/>
       <c r="M95" s="12"/>
@@ -5236,14 +5259,14 @@
       <c r="A96" s="3">
         <v>105</v>
       </c>
-      <c r="B96" s="29" t="s">
-        <v>128</v>
+      <c r="B96" s="28" t="s">
+        <v>133</v>
       </c>
       <c r="C96" s="12"/>
       <c r="D96" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E96" s="16" t="s">
+      <c r="E96" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F96" s="12" t="s">
@@ -5258,7 +5281,7 @@
       <c r="I96" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J96" s="24"/>
+      <c r="J96" s="23"/>
       <c r="K96" s="12"/>
       <c r="L96" s="12"/>
       <c r="M96" s="12"/>
@@ -5272,14 +5295,14 @@
       <c r="A97" s="3">
         <v>106</v>
       </c>
-      <c r="B97" s="29" t="s">
-        <v>129</v>
+      <c r="B97" s="28" t="s">
+        <v>134</v>
       </c>
       <c r="C97" s="12"/>
       <c r="D97" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E97" s="16" t="s">
+      <c r="E97" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F97" s="12" t="s">
@@ -5294,7 +5317,7 @@
       <c r="I97" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J97" s="24"/>
+      <c r="J97" s="23"/>
       <c r="K97" s="12"/>
       <c r="L97" s="12"/>
       <c r="M97" s="12"/>
@@ -5308,14 +5331,14 @@
       <c r="A98" s="3">
         <v>107</v>
       </c>
-      <c r="B98" s="29" t="s">
-        <v>130</v>
+      <c r="B98" s="28" t="s">
+        <v>135</v>
       </c>
       <c r="C98" s="12"/>
       <c r="D98" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E98" s="16" t="s">
+      <c r="E98" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F98" s="12" t="s">
@@ -5330,7 +5353,7 @@
       <c r="I98" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J98" s="24"/>
+      <c r="J98" s="23"/>
       <c r="K98" s="12"/>
       <c r="L98" s="12"/>
       <c r="M98" s="12"/>
@@ -5345,13 +5368,13 @@
         <v>108</v>
       </c>
       <c r="B99" s="30" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C99" s="12"/>
       <c r="D99" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E99" s="16" t="s">
+      <c r="E99" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F99" s="12" t="s">
@@ -5366,7 +5389,7 @@
       <c r="I99" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J99" s="24"/>
+      <c r="J99" s="23"/>
       <c r="K99" s="12"/>
       <c r="L99" s="12"/>
       <c r="M99" s="12"/>
@@ -5381,13 +5404,13 @@
         <v>109</v>
       </c>
       <c r="B100" s="30" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="C100" s="12"/>
       <c r="D100" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E100" s="16" t="s">
+      <c r="E100" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F100" s="12" t="s">
@@ -5402,7 +5425,7 @@
       <c r="I100" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J100" s="24"/>
+      <c r="J100" s="23"/>
       <c r="K100" s="12"/>
       <c r="L100" s="12"/>
       <c r="M100" s="12"/>
@@ -5417,13 +5440,13 @@
         <v>110</v>
       </c>
       <c r="B101" s="30" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="C101" s="12"/>
       <c r="D101" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E101" s="16" t="s">
+      <c r="E101" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F101" s="12" t="s">
@@ -5438,7 +5461,7 @@
       <c r="I101" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J101" s="24"/>
+      <c r="J101" s="23"/>
       <c r="K101" s="12"/>
       <c r="L101" s="12"/>
       <c r="M101" s="12"/>
@@ -5453,13 +5476,13 @@
         <v>111</v>
       </c>
       <c r="B102" s="30" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="C102" s="12"/>
       <c r="D102" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E102" s="16" t="s">
+      <c r="E102" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F102" s="12" t="s">
@@ -5474,7 +5497,7 @@
       <c r="I102" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J102" s="24"/>
+      <c r="J102" s="23"/>
       <c r="K102" s="12"/>
       <c r="L102" s="12"/>
       <c r="M102" s="12"/>
@@ -5489,13 +5512,13 @@
         <v>112</v>
       </c>
       <c r="B103" s="30" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="C103" s="12"/>
       <c r="D103" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E103" s="16" t="s">
+      <c r="E103" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F103" s="12" t="s">
@@ -5510,7 +5533,7 @@
       <c r="I103" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J103" s="24"/>
+      <c r="J103" s="23"/>
       <c r="K103" s="12"/>
       <c r="L103" s="12"/>
       <c r="M103" s="12"/>
@@ -5525,13 +5548,13 @@
         <v>113</v>
       </c>
       <c r="B104" s="30" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="C104" s="12"/>
       <c r="D104" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E104" s="16" t="s">
+      <c r="E104" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F104" s="12" t="s">
@@ -5546,7 +5569,7 @@
       <c r="I104" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J104" s="24"/>
+      <c r="J104" s="23"/>
       <c r="K104" s="12"/>
       <c r="L104" s="12"/>
       <c r="M104" s="12"/>
@@ -5561,13 +5584,13 @@
         <v>114</v>
       </c>
       <c r="B105" s="30" t="s">
-        <v>137</v>
+        <v>142</v>
       </c>
       <c r="C105" s="12"/>
       <c r="D105" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E105" s="16" t="s">
+      <c r="E105" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F105" s="12" t="s">
@@ -5582,7 +5605,7 @@
       <c r="I105" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J105" s="24"/>
+      <c r="J105" s="23"/>
       <c r="K105" s="12"/>
       <c r="L105" s="12"/>
       <c r="M105" s="12"/>
@@ -5597,13 +5620,13 @@
         <v>115</v>
       </c>
       <c r="B106" s="30" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C106" s="12"/>
       <c r="D106" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E106" s="16" t="s">
+      <c r="E106" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F106" s="12" t="s">
@@ -5618,7 +5641,7 @@
       <c r="I106" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J106" s="24"/>
+      <c r="J106" s="23"/>
       <c r="K106" s="12"/>
       <c r="L106" s="12"/>
       <c r="M106" s="12"/>
@@ -5633,13 +5656,13 @@
         <v>116</v>
       </c>
       <c r="B107" s="30" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
       <c r="C107" s="12"/>
       <c r="D107" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E107" s="16" t="s">
+      <c r="E107" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F107" s="12" t="s">
@@ -5654,7 +5677,7 @@
       <c r="I107" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J107" s="24"/>
+      <c r="J107" s="23"/>
       <c r="K107" s="12"/>
       <c r="L107" s="12"/>
       <c r="M107" s="12"/>
@@ -5669,13 +5692,13 @@
         <v>117</v>
       </c>
       <c r="B108" s="30" t="s">
-        <v>140</v>
+        <v>145</v>
       </c>
       <c r="C108" s="12"/>
       <c r="D108" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E108" s="16" t="s">
+      <c r="E108" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F108" s="12" t="s">
@@ -5690,7 +5713,7 @@
       <c r="I108" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J108" s="24"/>
+      <c r="J108" s="23"/>
       <c r="K108" s="12"/>
       <c r="L108" s="12"/>
       <c r="M108" s="12"/>
@@ -5705,13 +5728,13 @@
         <v>118</v>
       </c>
       <c r="B109" s="30" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="C109" s="12"/>
       <c r="D109" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E109" s="16" t="s">
+      <c r="E109" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F109" s="12" t="s">
@@ -5726,7 +5749,7 @@
       <c r="I109" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J109" s="24"/>
+      <c r="J109" s="23"/>
       <c r="K109" s="12"/>
       <c r="L109" s="12"/>
       <c r="M109" s="12"/>
@@ -5741,13 +5764,13 @@
         <v>119</v>
       </c>
       <c r="B110" s="30" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
       <c r="C110" s="12"/>
       <c r="D110" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="E110" s="16" t="s">
+      <c r="E110" s="15" t="s">
         <v>21</v>
       </c>
       <c r="F110" s="12" t="s">
@@ -5762,7 +5785,7 @@
       <c r="I110" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J110" s="24"/>
+      <c r="J110" s="23"/>
       <c r="K110" s="12"/>
       <c r="L110" s="12"/>
       <c r="M110" s="12"/>
@@ -5777,7 +5800,7 @@
         <v>120</v>
       </c>
       <c r="B111" s="30" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="C111" s="12"/>
       <c r="D111" s="11" t="s">
@@ -5798,7 +5821,7 @@
       <c r="I111" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J111" s="24"/>
+      <c r="J111" s="23"/>
       <c r="K111" s="12"/>
       <c r="L111" s="12"/>
       <c r="M111" s="12"/>
@@ -5813,7 +5836,7 @@
         <v>121</v>
       </c>
       <c r="B112" s="30" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="C112" s="12"/>
       <c r="D112" s="11" t="s">
@@ -5834,7 +5857,7 @@
       <c r="I112" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J112" s="24"/>
+      <c r="J112" s="23"/>
       <c r="K112" s="12"/>
       <c r="L112" s="12"/>
       <c r="M112" s="12"/>
@@ -5849,7 +5872,7 @@
         <v>122</v>
       </c>
       <c r="B113" s="30" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="C113" s="12"/>
       <c r="D113" s="11" t="s">
@@ -5870,7 +5893,7 @@
       <c r="I113" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J113" s="24"/>
+      <c r="J113" s="23"/>
       <c r="K113" s="12"/>
       <c r="L113" s="12"/>
       <c r="M113" s="12"/>
@@ -5885,7 +5908,7 @@
         <v>123</v>
       </c>
       <c r="B114" s="30" t="s">
-        <v>146</v>
+        <v>151</v>
       </c>
       <c r="C114" s="12"/>
       <c r="D114" s="11" t="s">
@@ -5906,7 +5929,7 @@
       <c r="I114" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J114" s="24"/>
+      <c r="J114" s="23"/>
       <c r="K114" s="12"/>
       <c r="L114" s="12"/>
       <c r="M114" s="12"/>
@@ -5921,7 +5944,7 @@
         <v>124</v>
       </c>
       <c r="B115" s="31" t="s">
-        <v>147</v>
+        <v>152</v>
       </c>
       <c r="C115" s="12"/>
       <c r="D115" s="11" t="s">
@@ -5942,7 +5965,7 @@
       <c r="I115" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J115" s="24"/>
+      <c r="J115" s="23"/>
       <c r="K115" s="12"/>
       <c r="L115" s="12"/>
       <c r="M115" s="12"/>
@@ -5957,7 +5980,7 @@
         <v>125</v>
       </c>
       <c r="B116" s="31" t="s">
-        <v>148</v>
+        <v>153</v>
       </c>
       <c r="C116" s="12"/>
       <c r="D116" s="11" t="s">
@@ -5978,7 +6001,7 @@
       <c r="I116" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J116" s="24"/>
+      <c r="J116" s="23"/>
       <c r="K116" s="12"/>
       <c r="L116" s="12"/>
       <c r="M116" s="12"/>
@@ -5993,10 +6016,10 @@
         <v>126</v>
       </c>
       <c r="B117" s="31" t="s">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C117" s="10" t="s">
-        <v>150</v>
+        <v>155</v>
       </c>
       <c r="D117" s="11" t="s">
         <v>13</v>
@@ -6016,7 +6039,7 @@
       <c r="I117" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J117" s="24"/>
+      <c r="J117" s="23"/>
       <c r="K117" s="12"/>
       <c r="L117" s="12"/>
       <c r="M117" s="12"/>
@@ -6031,10 +6054,10 @@
         <v>127</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C118" s="10" t="s">
-        <v>152</v>
+        <v>157</v>
       </c>
       <c r="D118" s="11" t="s">
         <v>13</v>
@@ -6054,7 +6077,7 @@
       <c r="I118" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J118" s="24"/>
+      <c r="J118" s="23"/>
       <c r="K118" s="12"/>
       <c r="L118" s="12"/>
       <c r="M118" s="12"/>
@@ -6069,10 +6092,10 @@
         <v>128</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>153</v>
+        <v>158</v>
       </c>
       <c r="C119" s="10" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="D119" s="11" t="s">
         <v>13</v>
@@ -6087,12 +6110,12 @@
         <v>35</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I119" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J119" s="24"/>
+      <c r="J119" s="23"/>
       <c r="K119" s="12"/>
       <c r="L119" s="12"/>
       <c r="M119" s="12"/>
@@ -6107,10 +6130,10 @@
         <v>129</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>156</v>
+        <v>161</v>
       </c>
       <c r="C120" s="10" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="D120" s="11" t="s">
         <v>13</v>
@@ -6125,12 +6148,12 @@
         <v>35</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="I120" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J120" s="24"/>
+      <c r="J120" s="23"/>
       <c r="K120" s="12"/>
       <c r="L120" s="12"/>
       <c r="M120" s="12"/>
@@ -6145,7 +6168,7 @@
         <v>130</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="C121" s="10"/>
       <c r="D121" s="11" t="s">
@@ -6166,7 +6189,7 @@
       <c r="I121" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J121" s="24"/>
+      <c r="J121" s="23"/>
       <c r="K121" s="12"/>
       <c r="L121" s="12"/>
       <c r="M121" s="12"/>
@@ -6181,7 +6204,7 @@
         <v>131</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="C122" s="12"/>
       <c r="D122" s="11" t="s">
@@ -6202,7 +6225,7 @@
       <c r="I122" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J122" s="24"/>
+      <c r="J122" s="23"/>
       <c r="K122" s="12"/>
       <c r="L122" s="12"/>
       <c r="M122" s="12"/>
@@ -6217,7 +6240,7 @@
         <v>132</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="C123" s="12"/>
       <c r="D123" s="11" t="s">
@@ -6238,7 +6261,7 @@
       <c r="I123" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J123" s="24"/>
+      <c r="J123" s="23"/>
       <c r="K123" s="12"/>
       <c r="L123" s="12"/>
       <c r="M123" s="12"/>
@@ -6253,7 +6276,7 @@
         <v>133</v>
       </c>
       <c r="B124" s="31" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C124" s="12"/>
       <c r="D124" s="11" t="s">
@@ -6274,7 +6297,7 @@
       <c r="I124" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J124" s="24"/>
+      <c r="J124" s="23"/>
       <c r="K124" s="12"/>
       <c r="L124" s="12"/>
       <c r="M124" s="12"/>
@@ -6289,7 +6312,7 @@
         <v>134</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>162</v>
+        <v>167</v>
       </c>
       <c r="C125" s="12"/>
       <c r="D125" s="11" t="s">
@@ -6310,7 +6333,7 @@
       <c r="I125" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J125" s="24"/>
+      <c r="J125" s="23"/>
       <c r="K125" s="12"/>
       <c r="L125" s="12"/>
       <c r="M125" s="12"/>
@@ -6325,7 +6348,7 @@
         <v>135</v>
       </c>
       <c r="B126" s="31" t="s">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c r="C126" s="12"/>
       <c r="D126" s="11" t="s">
@@ -6346,7 +6369,7 @@
       <c r="I126" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J126" s="24"/>
+      <c r="J126" s="23"/>
       <c r="K126" s="12"/>
       <c r="L126" s="12"/>
       <c r="M126" s="12"/>
@@ -6361,7 +6384,7 @@
         <v>136</v>
       </c>
       <c r="B127" s="31" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c r="C127" s="12"/>
       <c r="D127" s="11" t="s">
@@ -6382,7 +6405,7 @@
       <c r="I127" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J127" s="24"/>
+      <c r="J127" s="23"/>
       <c r="K127" s="12"/>
       <c r="L127" s="12"/>
       <c r="M127" s="12"/>
@@ -6397,7 +6420,7 @@
         <v>137</v>
       </c>
       <c r="B128" s="31" t="s">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c r="C128" s="12"/>
       <c r="D128" s="11" t="s">
@@ -6418,7 +6441,7 @@
       <c r="I128" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J128" s="24"/>
+      <c r="J128" s="23"/>
       <c r="K128" s="12"/>
       <c r="L128" s="12"/>
       <c r="M128" s="12"/>
@@ -6433,7 +6456,7 @@
         <v>138</v>
       </c>
       <c r="B129" s="31" t="s">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c r="C129" s="12"/>
       <c r="D129" s="11" t="s">
@@ -6454,7 +6477,7 @@
       <c r="I129" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J129" s="24"/>
+      <c r="J129" s="23"/>
       <c r="K129" s="12"/>
       <c r="L129" s="12"/>
       <c r="M129" s="12"/>
@@ -6469,7 +6492,7 @@
         <v>139</v>
       </c>
       <c r="B130" s="31" t="s">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="C130" s="12"/>
       <c r="D130" s="11" t="s">
@@ -6490,7 +6513,7 @@
       <c r="I130" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J130" s="24"/>
+      <c r="J130" s="23"/>
       <c r="K130" s="12"/>
       <c r="L130" s="12"/>
       <c r="M130" s="12"/>
@@ -6505,7 +6528,7 @@
         <v>140</v>
       </c>
       <c r="B131" s="32" t="s">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="C131" s="12"/>
       <c r="D131" s="11" t="s">
@@ -6526,7 +6549,7 @@
       <c r="I131" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J131" s="24"/>
+      <c r="J131" s="23"/>
       <c r="K131" s="12"/>
       <c r="L131" s="12"/>
       <c r="M131" s="12"/>
@@ -6541,7 +6564,7 @@
         <v>141</v>
       </c>
       <c r="B132" s="32" t="s">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c r="C132" s="12"/>
       <c r="D132" s="11" t="s">
@@ -6562,7 +6585,7 @@
       <c r="I132" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J132" s="24"/>
+      <c r="J132" s="23"/>
       <c r="K132" s="12"/>
       <c r="L132" s="12"/>
       <c r="M132" s="12"/>
@@ -6577,7 +6600,7 @@
         <v>142</v>
       </c>
       <c r="B133" s="32" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="C133" s="12"/>
       <c r="D133" s="11" t="s">
@@ -6598,7 +6621,7 @@
       <c r="I133" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J133" s="24"/>
+      <c r="J133" s="23"/>
       <c r="K133" s="12"/>
       <c r="L133" s="12"/>
       <c r="M133" s="12"/>
@@ -6613,7 +6636,7 @@
         <v>143</v>
       </c>
       <c r="B134" s="32" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="C134" s="12"/>
       <c r="D134" s="11" t="s">
@@ -6634,7 +6657,7 @@
       <c r="I134" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J134" s="24"/>
+      <c r="J134" s="23"/>
       <c r="K134" s="12"/>
       <c r="L134" s="12"/>
       <c r="M134" s="12"/>
@@ -6649,7 +6672,7 @@
         <v>144</v>
       </c>
       <c r="B135" s="32" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="C135" s="12"/>
       <c r="D135" s="11" t="s">
@@ -6670,7 +6693,7 @@
       <c r="I135" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J135" s="24"/>
+      <c r="J135" s="23"/>
       <c r="K135" s="12"/>
       <c r="L135" s="12"/>
       <c r="M135" s="12"/>
@@ -6685,7 +6708,7 @@
         <v>145</v>
       </c>
       <c r="B136" s="32" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="C136" s="12"/>
       <c r="D136" s="11" t="s">
@@ -6706,7 +6729,7 @@
       <c r="I136" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J136" s="24"/>
+      <c r="J136" s="23"/>
       <c r="K136" s="12"/>
       <c r="L136" s="12"/>
       <c r="M136" s="12"/>
@@ -6721,7 +6744,7 @@
         <v>146</v>
       </c>
       <c r="B137" s="32" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="C137" s="12"/>
       <c r="D137" s="11" t="s">
@@ -6742,7 +6765,7 @@
       <c r="I137" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J137" s="24"/>
+      <c r="J137" s="23"/>
       <c r="K137" s="12"/>
       <c r="L137" s="12"/>
       <c r="M137" s="12"/>
@@ -6757,7 +6780,7 @@
         <v>147</v>
       </c>
       <c r="B138" s="32" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="C138" s="12"/>
       <c r="D138" s="11" t="s">
@@ -6778,7 +6801,7 @@
       <c r="I138" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J138" s="24"/>
+      <c r="J138" s="23"/>
       <c r="K138" s="12"/>
       <c r="L138" s="12"/>
       <c r="M138" s="12"/>
@@ -6793,7 +6816,7 @@
         <v>148</v>
       </c>
       <c r="B139" s="32" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="C139" s="12"/>
       <c r="D139" s="11" t="s">
@@ -6814,7 +6837,7 @@
       <c r="I139" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J139" s="24"/>
+      <c r="J139" s="23"/>
       <c r="K139" s="12"/>
       <c r="L139" s="12"/>
       <c r="M139" s="12"/>
@@ -6829,7 +6852,7 @@
         <v>149</v>
       </c>
       <c r="B140" s="32" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="C140" s="12"/>
       <c r="D140" s="11" t="s">
@@ -6850,7 +6873,7 @@
       <c r="I140" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J140" s="24"/>
+      <c r="J140" s="23"/>
       <c r="K140" s="12"/>
       <c r="L140" s="12"/>
       <c r="M140" s="12"/>
@@ -6865,7 +6888,7 @@
         <v>150</v>
       </c>
       <c r="B141" s="32" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="C141" s="12"/>
       <c r="D141" s="11" t="s">
@@ -6886,7 +6909,7 @@
       <c r="I141" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J141" s="24"/>
+      <c r="J141" s="23"/>
       <c r="K141" s="12"/>
       <c r="L141" s="12"/>
       <c r="M141" s="12"/>
@@ -6901,7 +6924,7 @@
         <v>151</v>
       </c>
       <c r="B142" s="32" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="C142" s="12"/>
       <c r="D142" s="11" t="s">
@@ -6922,7 +6945,7 @@
       <c r="I142" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J142" s="24"/>
+      <c r="J142" s="23"/>
       <c r="K142" s="12"/>
       <c r="L142" s="12"/>
       <c r="M142" s="12"/>
@@ -6933,7 +6956,7 @@
       <c r="R142" s="12"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:F91">
+  <autoFilter ref="A2:F142">
     <extLst/>
   </autoFilter>
   <mergeCells count="2">
@@ -6941,29 +6964,29 @@
     <mergeCell ref="K1:R1"/>
   </mergeCells>
   <dataValidations count="11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J91 J4:J90 R4:R91 J92:R142">
+      <formula1>"Low,High"</formula1>
+    </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H3 H4 H5 H6 H7 H8 H9 H10 H11 H14 H15 H16 H17 H18 H19 H20 H21 H22 H23 H24 H25 H26 H27 H28 H29 H30 H31 H32 H33 H34 H35 H36 H37 H38 H39 H40 H41 H42 H43 H44 H45 H46 H47 H48 H49 H50 H51 H52 H53 H54 H55 H56 H57 H58 H59 H60 H61 H62 H63 H64 H65 H66 H67 H68 H69 H70 H71 H72 H73 H74 H75 H76 H77 H78 H79 H80 H81 H82 H83 H84 H85 H86 H87 H88 H89 H90 H91 H92 H93 H94 H95 H96 H97 H98 H99 H100 H101 H102 H103 H104 H105 H106 H107 H108 H109 H110 H111 H112 H113 H114 H115 H116 H117 H118 H119 H120 H121 H122 H123 H124 H125 H126 H127 H128 H129 H130 H131 H132 H133 H134 H135 H136 H137 H138 H139 H140 H141 H142 H12:H13">
       <formula1>"GPIO_AF0,GPIO_AF1,GPIO_AF2,GPIO_AF3,GPIO_AF4,GPIO_AF5,GPIO_AF6,GPIO_AF7,GPIO_AF8,GPIO_AF9,GPIO_AF10,GPIO_AF11,GPIO_AF12,GPIO_AF13,GPIO_AF14,GPIO_AF15"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J91 J4:J90 R4:R91 J92:R142">
-      <formula1>"Low,High"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D90 D91:D142">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E51 E52:E110 E111:E142 K3:K91">
+      <formula1>"NoPull,PullDown,PullUp"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F3:F142">
       <formula1>"GPIO_MODE_INPUT,GPIO_MODE_OUTPUT_PP,GPIO_MODE_OUTPUT_OD,GPIO_MODE_AF_PP,GPIO_MODE_AF_OD"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D90 D91:D142">
-      <formula1>"Yes,No"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G3:G142">
+      <formula1>"GPIO_SPEED_LOW,GPIO_SPEED_MEDIUM,GPIO_SPEED_FAST,GPIO_SPEED_HIGH"</formula1>
+    </dataValidation>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L3:L91">
+      <formula1>"UnLock,Lock"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I90 I91:I142 Q3:Q91">
       <formula1>"Input,Low,High"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G3:G142">
-      <formula1>"GPIO_SPEED_LOW,GPIO_SPEED_MEDIUM,GPIO_SPEED_FAST,GPIO_SPEED_HIGH"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E51 E52:E110 E111:E142 K3:K91">
-      <formula1>"NoPull,PullDown,PullUp"</formula1>
-    </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="L3:L91">
-      <formula1>"UnLock,Lock"</formula1>
     </dataValidation>
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="M3:M91">
       <formula1>"None,LowDrive,HighDrive"</formula1>

</xml_diff>